<commit_message>
Update of the Gantt Chart
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testbctcstudent-my.sharepoint.com/personal/jusnun404_bctcstudent_org/Documents/Productivity Software/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\Senior_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{09B506CF-F528-4441-8001-8EF6DBDEC203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AC38A3C-3C3E-4C17-9C1C-F9343C063D71}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8288D61C-655E-4463-B08B-3AFC9A173158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{D2CA3B49-F37C-404E-8452-632B820BCCBE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Start Date</t>
   </si>
@@ -54,22 +54,61 @@
     <t>Design GUI</t>
   </si>
   <si>
-    <t>Design Code</t>
-  </si>
-  <si>
-    <t>Phase 1 Coding</t>
-  </si>
-  <si>
-    <t>Phase 2 Coding</t>
-  </si>
-  <si>
-    <t>Testing Phase</t>
-  </si>
-  <si>
-    <t>Fix Phase</t>
-  </si>
-  <si>
-    <t>Phase 3 Coding</t>
+    <t>Phase Name</t>
+  </si>
+  <si>
+    <t>Code the schedule function and program lock function</t>
+  </si>
+  <si>
+    <t>Code the usages times function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research </t>
+  </si>
+  <si>
+    <t>Fix</t>
+  </si>
+  <si>
+    <t>Fix all the possible errors that the program may have</t>
+  </si>
+  <si>
+    <t>Second and Third Function</t>
+  </si>
+  <si>
+    <t>First Function</t>
+  </si>
+  <si>
+    <t>GUI Skeleton</t>
+  </si>
+  <si>
+    <t>Code GUI skeleton to start adding the functions to the program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalize the GUI </t>
+  </si>
+  <si>
+    <t>Add the Themes to the GUI, and stylize it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desing </t>
+  </si>
+  <si>
+    <t>Test the 2 last functions, and if the have errors correct it.</t>
+  </si>
+  <si>
+    <t>Test the first function and if have errors correct it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Test </t>
+  </si>
+  <si>
+    <t>Test the program in its entirety and give it as a beta program to some selected users with the purpose of testing it</t>
+  </si>
+  <si>
+    <t>Individual Testing / Fix</t>
+  </si>
+  <si>
+    <t>Functions Testing /Fix</t>
   </si>
 </sst>
 </file>
@@ -152,12 +191,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -222,42 +265,48 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$4:$E$11</c:f>
+              <c:f>Sheet1!$E$4:$E$13</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Research Phase</c:v>
+                  <c:v>Research </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Design GUI</c:v>
+                  <c:v>Desing </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Design Code</c:v>
+                  <c:v>GUI Skeleton</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Phase 1 Coding</c:v>
+                  <c:v>First Function</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Phase 2 Coding</c:v>
+                  <c:v>Individual Testing / Fix</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Phase 3 Coding</c:v>
+                  <c:v>Second and Third Function</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Testing Phase</c:v>
+                  <c:v>Functions Testing /Fix</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Fix Phase</c:v>
+                  <c:v>Finalize the GUI </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>User Test </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Fix</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$11</c:f>
+              <c:f>Sheet1!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>44472</c:v>
                 </c:pt>
@@ -265,21 +314,27 @@
                   <c:v>44500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44522</c:v>
+                  <c:v>44514</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>44532</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>44544</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>44557</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>44564</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>44585</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>44619</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>44557</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>44627</c:v>
                 </c:pt>
               </c:numCache>
@@ -296,7 +351,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$3</c:f>
+              <c:f>Sheet1!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -317,64 +372,76 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$4:$E$11</c:f>
+              <c:f>Sheet1!$E$4:$E$13</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Research Phase</c:v>
+                  <c:v>Research </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Design GUI</c:v>
+                  <c:v>Desing </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Design Code</c:v>
+                  <c:v>GUI Skeleton</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Phase 1 Coding</c:v>
+                  <c:v>First Function</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Phase 2 Coding</c:v>
+                  <c:v>Individual Testing / Fix</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Phase 3 Coding</c:v>
+                  <c:v>Second and Third Function</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Testing Phase</c:v>
+                  <c:v>Functions Testing /Fix</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Fix Phase</c:v>
+                  <c:v>Finalize the GUI </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>User Test </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Fix</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$11</c:f>
+              <c:f>Sheet1!$G$4:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -1125,13 +1192,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>157528</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>165588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>365613</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>51288</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1457,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F41711F-647E-45BD-B0D2-B131E9E587E9}">
-  <dimension ref="C3:F11"/>
+  <dimension ref="C3:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,11 +1535,12 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="103.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1480,27 +1548,34 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C4" s="4">
         <v>44472</v>
       </c>
       <c r="D4" s="1">
-        <v>44499</v>
+        <v>44607</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2">
-        <v>27</v>
+      <c r="G4" s="2">
+        <f>_xlfn.DAYS(D4,C4)</f>
+        <v>135</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="4">
         <v>44500</v>
       </c>
@@ -1508,27 +1583,35 @@
         <v>44520</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G13" si="0">_xlfn.DAYS(D5,C5)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
-        <v>44522</v>
+        <v>44514</v>
       </c>
       <c r="D6" s="1">
-        <v>11658</v>
+        <v>44531</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="4">
         <v>44532</v>
       </c>
@@ -1536,65 +1619,121 @@
         <v>44555</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="4">
+        <v>44544</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44557</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="4">
+        <v>44557</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44582</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <v>23</v>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="4">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="4">
+        <v>44564</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44588</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="4">
+        <v>44585</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44613</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="4">
         <v>44557</v>
       </c>
-      <c r="D8" s="1">
-        <v>44582</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2">
-        <v>25</v>
+      <c r="D12" s="1">
+        <v>44625</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>68</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="4">
-        <v>44585</v>
-      </c>
-      <c r="D9" s="1">
-        <v>44613</v>
-      </c>
-      <c r="E9" s="2" t="s">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="4">
+        <v>44627</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44635</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="4">
-        <v>44619</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44625</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="4">
-        <v>44627</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44635</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>

</xml_diff>